<commit_message>
1) removed if?then:else, restructured the code and added comments 2) added test cases for Mixed Case, Upper Case and Lower Case. Both positive and negative tests are used 3) added files generated at build time in the commit
</commit_message>
<xml_diff>
--- a/test/test614.xlsx
+++ b/test/test614.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ACCount</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
   </si>
 </sst>
 </file>
@@ -358,22 +367,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>